<commit_message>
Modified my schedule and created 2 new files.
</commit_message>
<xml_diff>
--- a/2020-2021 1st semester schedule.xlsx
+++ b/2020-2021 1st semester schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\MySchedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F97D9F8-42D4-424B-84C5-76726B92B4A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6DA7D18-2173-4D8F-AAB2-D8387689D770}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="104">
   <si>
     <t>刘锐教师课表</t>
   </si>
@@ -185,6 +185,147 @@
   </si>
   <si>
     <t>主楼-108*</t>
+  </si>
+  <si>
+    <t>3-4</t>
+  </si>
+  <si>
+    <t>电工2</t>
+  </si>
+  <si>
+    <t>1南-507*</t>
+  </si>
+  <si>
+    <t>5-6</t>
+  </si>
+  <si>
+    <t>7-8</t>
+  </si>
+  <si>
+    <t>9-10</t>
+  </si>
+  <si>
+    <t>DG7,9</t>
+  </si>
+  <si>
+    <t>数字4</t>
+  </si>
+  <si>
+    <t>嘉园-203B</t>
+  </si>
+  <si>
+    <t>11-12</t>
+  </si>
+  <si>
+    <t>∞</t>
+  </si>
+  <si>
+    <t>二</t>
+  </si>
+  <si>
+    <t>网络5</t>
+  </si>
+  <si>
+    <t>1南-208*</t>
+  </si>
+  <si>
+    <t>通信3</t>
+  </si>
+  <si>
+    <t>1南-208*;主楼-507*</t>
+  </si>
+  <si>
+    <t>电工1</t>
+  </si>
+  <si>
+    <t>主楼-506*</t>
+  </si>
+  <si>
+    <t>三</t>
+  </si>
+  <si>
+    <t>1南-406*</t>
+  </si>
+  <si>
+    <t>DG1</t>
+  </si>
+  <si>
+    <t>DG3</t>
+  </si>
+  <si>
+    <t>DG1,3</t>
+  </si>
+  <si>
+    <t>四</t>
+  </si>
+  <si>
+    <t>DG7</t>
+  </si>
+  <si>
+    <t>1南-202*</t>
+  </si>
+  <si>
+    <t>1南-202*;嘉园-203B</t>
+  </si>
+  <si>
+    <t>1南-406*;嘉园-203B</t>
+  </si>
+  <si>
+    <t>DG9</t>
+  </si>
+  <si>
+    <t>五</t>
+  </si>
+  <si>
+    <t>元旦节</t>
+  </si>
+  <si>
+    <t>主楼-306*</t>
+  </si>
+  <si>
+    <t>1南-504*</t>
+  </si>
+  <si>
+    <t>六</t>
+  </si>
+  <si>
+    <t>CET4</t>
+  </si>
+  <si>
+    <t>CET6</t>
+  </si>
+  <si>
+    <t>日</t>
+  </si>
+  <si>
+    <t>理论课程</t>
+  </si>
+  <si>
+    <t>实验课程</t>
+  </si>
+  <si>
+    <t>开会/活动/冲突</t>
+  </si>
+  <si>
+    <t>监考/巡考/答疑</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>注：1.课程表中符号"∝"为三节连上课程，符号"∞"为四节连上课程.2.教室后有"*"的教室为多媒体教室</t>
+  </si>
+  <si>
+    <t>答疑</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX2</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>1-电工技术与电子技术C(56/3.5)(220160/刘锐/讲师)
@@ -202,148 +343,18 @@
 DG1--材料19-1
 DG3--材料19-3
 DG7--机械19-4
-DG9--机械19-6</t>
-  </si>
-  <si>
-    <t>3-4</t>
-  </si>
-  <si>
-    <t>电工2</t>
-  </si>
-  <si>
-    <t>1南-507*</t>
-  </si>
-  <si>
-    <t>5-6</t>
-  </si>
-  <si>
-    <t>7-8</t>
-  </si>
-  <si>
-    <t>9-10</t>
-  </si>
-  <si>
-    <t>DG7,9</t>
-  </si>
-  <si>
-    <t>数字4</t>
-  </si>
-  <si>
-    <t>嘉园-203B</t>
-  </si>
-  <si>
-    <t>11-12</t>
-  </si>
-  <si>
-    <t>∞</t>
-  </si>
-  <si>
-    <t>二</t>
-  </si>
-  <si>
-    <t>网络5</t>
-  </si>
-  <si>
-    <t>1南-208*</t>
-  </si>
-  <si>
-    <t>通信3</t>
-  </si>
-  <si>
-    <t>1南-208*;主楼-507*</t>
-  </si>
-  <si>
-    <t>电工1</t>
-  </si>
-  <si>
-    <t>主楼-506*</t>
-  </si>
-  <si>
-    <t>三</t>
-  </si>
-  <si>
-    <t>1南-406*</t>
-  </si>
-  <si>
-    <t>DG1</t>
-  </si>
-  <si>
-    <t>DG3</t>
-  </si>
-  <si>
-    <t>DG1,3</t>
-  </si>
-  <si>
-    <t>四</t>
-  </si>
-  <si>
-    <t>DG7</t>
-  </si>
-  <si>
-    <t>1南-202*</t>
-  </si>
-  <si>
-    <t>1南-202*;嘉园-203B</t>
-  </si>
-  <si>
-    <t>1南-406*;嘉园-203B</t>
-  </si>
-  <si>
-    <t>DG9</t>
-  </si>
-  <si>
-    <t>五</t>
-  </si>
-  <si>
-    <t>元旦节</t>
-  </si>
-  <si>
-    <t>主楼-306*</t>
-  </si>
-  <si>
-    <t>1南-504*</t>
-  </si>
-  <si>
-    <t>六</t>
-  </si>
-  <si>
-    <t>CET4</t>
-  </si>
-  <si>
-    <t>CET6</t>
-  </si>
-  <si>
-    <t>日</t>
-  </si>
-  <si>
-    <t>理论课程</t>
-  </si>
-  <si>
-    <t>实验课程</t>
-  </si>
-  <si>
-    <t>开会/活动/冲突</t>
-  </si>
-  <si>
-    <t>监考/巡考/答疑</t>
-  </si>
-  <si>
-    <t>DONE</t>
-  </si>
-  <si>
-    <t>注：1.课程表中符号"∝"为三节连上课程，符号"∞"为四节连上课程.2.教室后有"*"的教室为多媒体教室</t>
-  </si>
-  <si>
-    <t>答疑</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+DG9--机械19-6
+TX1--信息18-1
+TX2--信息18-2</t>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>TX1</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
     <t>TX2</t>
-    <phoneticPr fontId="8" type="noConversion"/>
+    <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -382,11 +393,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
-      <name val="黑体"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="等线"/>
@@ -401,6 +407,12 @@
     <font>
       <sz val="10"/>
       <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="黑体"/>
       <family val="3"/>
       <charset val="134"/>
     </font>
@@ -516,11 +528,11 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -558,13 +570,19 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -595,9 +613,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -879,74 +894,76 @@
   <dimension ref="A1:X47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K24" activeCellId="1" sqref="K20 K24"/>
+      <selection activeCell="N12" activeCellId="4" sqref="M24 M26:M27 M29 M32 N12:N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="22" width="6" customWidth="1"/>
+    <col min="2" max="2" width="6" customWidth="1"/>
+    <col min="3" max="6" width="6" hidden="1" customWidth="1"/>
+    <col min="7" max="22" width="6" customWidth="1"/>
     <col min="23" max="23" width="20.42578125" customWidth="1"/>
     <col min="24" max="24" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="20" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="14"/>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="14"/>
-      <c r="N1" s="14"/>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-      <c r="U1" s="14"/>
-      <c r="V1" s="14"/>
-      <c r="W1" s="14"/>
-      <c r="X1" s="14"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
     </row>
     <row r="2" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="22" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16"/>
+      <c r="L2" s="16"/>
+      <c r="M2" s="24" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="14"/>
-      <c r="O2" s="14"/>
-      <c r="P2" s="14"/>
-      <c r="Q2" s="14"/>
-      <c r="R2" s="14"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
-      <c r="U2" s="14"/>
-      <c r="V2" s="14"/>
-      <c r="W2" s="14"/>
-      <c r="X2" s="14"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
     </row>
     <row r="3" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1097,7 +1114,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="16" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1115,7 +1132,7 @@
       <c r="F5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="16" t="s">
         <v>53</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -1130,7 +1147,9 @@
       <c r="K5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="L5" s="1"/>
+      <c r="L5" s="13" t="s">
+        <v>102</v>
+      </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
@@ -1144,18 +1163,18 @@
       <c r="W5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="X5" s="15" t="s">
+      <c r="X5" s="17" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="16"/>
+      <c r="B6" s="1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="14"/>
-      <c r="B6" s="1" t="s">
+      <c r="C6" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C6" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="D6" s="4" t="s">
         <v>52</v>
       </c>
@@ -1165,11 +1184,11 @@
       <c r="F6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I6" s="4" t="s">
         <v>52</v>
@@ -1192,31 +1211,33 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
       <c r="W6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="X6" s="16"/>
+    </row>
+    <row r="7" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="16"/>
+      <c r="B7" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="X6" s="14"/>
-    </row>
-    <row r="7" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="14"/>
-      <c r="B7" s="1" t="s">
-        <v>59</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="G7" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G7" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="13" t="s">
-        <v>100</v>
-      </c>
-      <c r="L7" s="1"/>
+        <v>99</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>103</v>
+      </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
@@ -1228,20 +1249,20 @@
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
-      <c r="X7" s="14"/>
+      <c r="X7" s="16"/>
     </row>
     <row r="8" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="14"/>
+      <c r="A8" s="16"/>
       <c r="B8" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="G8" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H8" s="1"/>
@@ -1260,18 +1281,18 @@
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
-      <c r="X8" s="14"/>
+      <c r="X8" s="16"/>
     </row>
     <row r="9" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="14"/>
+      <c r="A9" s="16"/>
       <c r="B9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H9" s="6"/>
@@ -1280,12 +1301,10 @@
       <c r="K9" s="6"/>
       <c r="L9" s="6"/>
       <c r="M9" s="6"/>
-      <c r="N9" s="18" t="s">
-        <v>62</v>
-      </c>
+      <c r="N9" s="15"/>
       <c r="O9" s="1"/>
       <c r="P9" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q9" s="5" t="s">
         <v>52</v>
@@ -1296,20 +1315,20 @@
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="X9" s="16"/>
+    </row>
+    <row r="10" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="16"/>
+      <c r="B10" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="X9" s="14"/>
-    </row>
-    <row r="10" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="14"/>
-      <c r="B10" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="1"/>
@@ -1318,13 +1337,13 @@
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
-      <c r="N10" s="19"/>
+      <c r="N10" s="15"/>
       <c r="O10" s="1"/>
       <c r="P10" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q10" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
@@ -1332,13 +1351,13 @@
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="X10" s="14"/>
+        <v>63</v>
+      </c>
+      <c r="X10" s="16"/>
     </row>
     <row r="11" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="14" t="s">
-        <v>67</v>
+      <c r="A11" s="16" t="s">
+        <v>66</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>50</v>
@@ -1347,19 +1366,19 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="M11" s="5" t="s">
+      <c r="K11" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M11" s="4" t="s">
         <v>52</v>
       </c>
       <c r="N11" s="6"/>
@@ -1372,33 +1391,33 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
       <c r="W11" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="X11" s="14"/>
+        <v>57</v>
+      </c>
+      <c r="X11" s="16"/>
     </row>
     <row r="12" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="14"/>
+      <c r="A12" s="16"/>
       <c r="B12" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
-      <c r="L12" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="N12" s="5" t="s">
+      <c r="L12" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="N12" s="4" t="s">
         <v>52</v>
       </c>
       <c r="O12" s="5" t="s">
@@ -1422,47 +1441,47 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
       <c r="W12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="X12" s="16"/>
+    </row>
+    <row r="13" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="16"/>
+      <c r="B13" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="G13" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="K13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L13" s="1"/>
+      <c r="M13" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="X12" s="14"/>
-    </row>
-    <row r="13" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="14"/>
-      <c r="B13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="H13" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="I13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="K13" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="N13" s="5" t="s">
+      <c r="N13" s="4" t="s">
         <v>52</v>
       </c>
       <c r="O13" s="5" t="s">
@@ -1484,18 +1503,18 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
       <c r="W13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="X13" s="16"/>
+    </row>
+    <row r="14" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="16"/>
+      <c r="B14" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C14" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="X13" s="14"/>
-    </row>
-    <row r="14" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="14"/>
-      <c r="B14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C14" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="D14" s="4" t="s">
         <v>52</v>
       </c>
@@ -1505,11 +1524,11 @@
       <c r="F14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="G14" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>52</v>
@@ -1517,13 +1536,13 @@
       <c r="J14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K14" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L14" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="M14" s="5" t="s">
+      <c r="K14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M14" s="4" t="s">
         <v>52</v>
       </c>
       <c r="N14" s="1"/>
@@ -1536,29 +1555,29 @@
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
       <c r="W14" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="X14" s="14"/>
+        <v>72</v>
+      </c>
+      <c r="X14" s="16"/>
     </row>
     <row r="15" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="14"/>
+      <c r="A15" s="16"/>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="14" t="s">
+      <c r="G15" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
-      <c r="K15" s="18" t="s">
-        <v>62</v>
-      </c>
-      <c r="L15" s="1"/>
+      <c r="K15" s="14"/>
+      <c r="L15" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
@@ -1570,25 +1589,25 @@
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
-      <c r="X15" s="14"/>
+      <c r="X15" s="16"/>
     </row>
     <row r="16" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="14"/>
+      <c r="A16" s="16"/>
       <c r="B16" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="14" t="s">
+      <c r="G16" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="1"/>
+      <c r="K16" s="14"/>
+      <c r="L16" s="19"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1600,11 +1619,11 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
-      <c r="X16" s="14"/>
+      <c r="X16" s="16"/>
     </row>
     <row r="17" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="14" t="s">
-        <v>74</v>
+      <c r="A17" s="16" t="s">
+        <v>73</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>50</v>
@@ -1613,7 +1632,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="14" t="s">
+      <c r="G17" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H17" s="1"/>
@@ -1632,12 +1651,12 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
-      <c r="X17" s="14"/>
+      <c r="X17" s="16"/>
     </row>
     <row r="18" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="14"/>
+      <c r="A18" s="16"/>
       <c r="B18" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>51</v>
@@ -1651,7 +1670,7 @@
       <c r="F18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="G18" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H18" s="4" t="s">
@@ -1663,7 +1682,7 @@
       <c r="J18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K18" s="5" t="s">
+      <c r="K18" s="4" t="s">
         <v>52</v>
       </c>
       <c r="L18" s="1"/>
@@ -1678,17 +1697,17 @@
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
       <c r="W18" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="X18" s="14"/>
+        <v>68</v>
+      </c>
+      <c r="X18" s="16"/>
     </row>
     <row r="19" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="14"/>
+      <c r="A19" s="16"/>
       <c r="B19" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>52</v>
@@ -1699,11 +1718,11 @@
       <c r="F19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I19" s="4" t="s">
         <v>52</v>
@@ -1711,13 +1730,13 @@
       <c r="J19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K19" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L19" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="M19" s="5" t="s">
+      <c r="K19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L19" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M19" s="4" t="s">
         <v>52</v>
       </c>
       <c r="N19" s="1"/>
@@ -1730,29 +1749,29 @@
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
       <c r="W19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="X19" s="14"/>
+        <v>74</v>
+      </c>
+      <c r="X19" s="16"/>
     </row>
     <row r="20" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="14"/>
+      <c r="A20" s="16"/>
       <c r="B20" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="14" t="s">
+      <c r="G20" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
-      <c r="K20" s="26" t="s">
-        <v>100</v>
+      <c r="K20" s="13" t="s">
+        <v>99</v>
       </c>
       <c r="L20" s="1"/>
       <c r="M20" s="1"/>
@@ -1766,38 +1785,38 @@
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
-      <c r="X20" s="14"/>
+      <c r="X20" s="16"/>
     </row>
     <row r="21" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="14"/>
+      <c r="A21" s="16"/>
       <c r="B21" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="H21" s="16" t="s">
+      <c r="G21" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="I21" s="18" t="s">
         <v>76</v>
-      </c>
-      <c r="I21" s="16" t="s">
-        <v>77</v>
       </c>
       <c r="J21" s="7"/>
       <c r="K21" s="18" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-      <c r="N21" s="18" t="s">
-        <v>78</v>
+      <c r="N21" s="20" t="s">
+        <v>77</v>
       </c>
       <c r="O21" s="1"/>
       <c r="P21" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q21" s="5" t="s">
         <v>52</v>
@@ -1808,35 +1827,35 @@
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="X21" s="16"/>
+    </row>
+    <row r="22" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="16"/>
+      <c r="B22" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="X21" s="14"/>
-    </row>
-    <row r="22" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="14"/>
-      <c r="B22" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="H22" s="17"/>
-      <c r="I22" s="17"/>
+      <c r="G22" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
       <c r="J22" s="7"/>
       <c r="K22" s="19"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-      <c r="N22" s="19"/>
+      <c r="N22" s="21"/>
       <c r="O22" s="1"/>
       <c r="P22" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q22" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
@@ -1844,30 +1863,30 @@
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="X22" s="14"/>
+        <v>63</v>
+      </c>
+      <c r="X22" s="16"/>
     </row>
     <row r="23" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="14" t="s">
-        <v>79</v>
+      <c r="A23" s="16" t="s">
+        <v>78</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="F23" s="14" t="s">
+      <c r="E23" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="F23" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>80</v>
+      <c r="G23" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>79</v>
       </c>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
@@ -1884,32 +1903,32 @@
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
-      <c r="X23" s="14"/>
+      <c r="X23" s="16"/>
     </row>
     <row r="24" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="14"/>
+      <c r="A24" s="16"/>
       <c r="B24" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="17"/>
-      <c r="F24" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="H24" s="17"/>
+      <c r="E24" s="19"/>
+      <c r="F24" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" s="19"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
-      <c r="K24" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="L24" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="M24" s="5" t="s">
+      <c r="K24" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="L24" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="M24" s="4" t="s">
         <v>52</v>
       </c>
       <c r="N24" s="5" t="s">
@@ -1936,14 +1955,14 @@
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
       <c r="W24" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="X24" s="14"/>
+        <v>80</v>
+      </c>
+      <c r="X24" s="16"/>
     </row>
     <row r="25" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="14"/>
+      <c r="A25" s="16"/>
       <c r="B25" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>51</v>
@@ -1954,10 +1973,10 @@
       <c r="E25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F25" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="14" t="s">
+      <c r="F25" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H25" s="4" t="s">
@@ -1969,7 +1988,7 @@
       <c r="J25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K25" s="5" t="s">
+      <c r="K25" s="4" t="s">
         <v>52</v>
       </c>
       <c r="L25" s="1"/>
@@ -1977,7 +1996,7 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q25" s="5" t="s">
         <v>52</v>
@@ -1988,17 +2007,17 @@
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
       <c r="W25" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="X25" s="14"/>
+        <v>81</v>
+      </c>
+      <c r="X25" s="16"/>
     </row>
     <row r="26" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="14"/>
+      <c r="A26" s="16"/>
       <c r="B26" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D26" s="4" t="s">
         <v>52</v>
@@ -2006,14 +2025,14 @@
       <c r="E26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F26" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26" s="14" t="s">
+      <c r="F26" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="16" t="s">
         <v>3</v>
       </c>
       <c r="H26" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>52</v>
@@ -2021,20 +2040,22 @@
       <c r="J26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K26" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="L26" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="M26" s="1"/>
+      <c r="K26" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="L26" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="M26" s="18" t="s">
+        <v>61</v>
+      </c>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q26" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
@@ -2042,41 +2063,41 @@
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
       <c r="W26" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="X26" s="14"/>
+        <v>82</v>
+      </c>
+      <c r="X26" s="16"/>
     </row>
     <row r="27" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="14"/>
+      <c r="A27" s="16"/>
       <c r="B27" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="16" t="s">
-        <v>84</v>
-      </c>
-      <c r="F27" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G27" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="H27" s="16" t="s">
-        <v>84</v>
+      <c r="E27" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="F27" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>83</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
+      <c r="M27" s="19"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q27" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
@@ -2084,25 +2105,25 @@
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
       <c r="W27" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="X27" s="16"/>
+    </row>
+    <row r="28" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="16"/>
+      <c r="B28" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="X27" s="14"/>
-    </row>
-    <row r="28" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="14"/>
-      <c r="B28" s="1" t="s">
-        <v>65</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="H28" s="17"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="19"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -2111,10 +2132,10 @@
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="Q28" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>
@@ -2122,13 +2143,13 @@
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
       <c r="W28" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="X28" s="14"/>
+        <v>63</v>
+      </c>
+      <c r="X28" s="16"/>
     </row>
     <row r="29" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="14" t="s">
-        <v>85</v>
+      <c r="A29" s="16" t="s">
+        <v>84</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>50</v>
@@ -2136,7 +2157,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G29" s="1"/>
@@ -2145,8 +2166,8 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="5" t="s">
-        <v>70</v>
+      <c r="M29" s="4" t="s">
+        <v>69</v>
       </c>
       <c r="N29" s="5" t="s">
         <v>52</v>
@@ -2163,36 +2184,36 @@
       <c r="R29" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="S29" s="14" t="s">
-        <v>86</v>
+      <c r="S29" s="16" t="s">
+        <v>85</v>
       </c>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
       <c r="W29" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="X29" s="14"/>
+        <v>86</v>
+      </c>
+      <c r="X29" s="16"/>
     </row>
     <row r="30" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="14"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C30" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="D30" s="4" t="s">
         <v>52</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="14" t="s">
+      <c r="F30" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H30" s="4" t="s">
         <v>52</v>
@@ -2203,7 +2224,7 @@
       <c r="J30" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="K30" s="5" t="s">
+      <c r="K30" s="4" t="s">
         <v>52</v>
       </c>
       <c r="L30" s="1"/>
@@ -2213,26 +2234,26 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
       <c r="R30" s="1"/>
-      <c r="S30" s="14" t="s">
+      <c r="S30" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
       <c r="W30" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="X30" s="14"/>
+        <v>87</v>
+      </c>
+      <c r="X30" s="16"/>
     </row>
     <row r="31" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="14"/>
+      <c r="A31" s="16"/>
       <c r="B31" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="14" t="s">
+      <c r="F31" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G31" s="1"/>
@@ -2247,24 +2268,24 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
       <c r="R31" s="1"/>
-      <c r="S31" s="14" t="s">
+      <c r="S31" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
-      <c r="X31" s="14"/>
+      <c r="X31" s="16"/>
     </row>
     <row r="32" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="14"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="14" t="s">
+      <c r="F32" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G32" s="1"/>
@@ -2272,10 +2293,10 @@
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
-      <c r="L32" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="M32" s="5" t="s">
+      <c r="L32" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="M32" s="4" t="s">
         <v>52</v>
       </c>
       <c r="N32" s="6"/>
@@ -2283,26 +2304,26 @@
       <c r="P32" s="6"/>
       <c r="Q32" s="6"/>
       <c r="R32" s="1"/>
-      <c r="S32" s="14" t="s">
+      <c r="S32" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T32" s="1"/>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="X32" s="14"/>
+        <v>87</v>
+      </c>
+      <c r="X32" s="16"/>
     </row>
     <row r="33" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="14"/>
+      <c r="A33" s="16"/>
       <c r="B33" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="14" t="s">
+      <c r="F33" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G33" s="1"/>
@@ -2317,24 +2338,24 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
-      <c r="S33" s="14" t="s">
+      <c r="S33" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
-      <c r="X33" s="14"/>
+      <c r="X33" s="16"/>
     </row>
     <row r="34" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="14"/>
+      <c r="A34" s="16"/>
       <c r="B34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G34" s="1"/>
@@ -2349,30 +2370,30 @@
       <c r="P34" s="1"/>
       <c r="Q34" s="1"/>
       <c r="R34" s="1"/>
-      <c r="S34" s="14" t="s">
+      <c r="S34" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
-      <c r="X34" s="14"/>
+      <c r="X34" s="16"/>
     </row>
     <row r="35" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="14" t="s">
-        <v>89</v>
+      <c r="A35" s="16" t="s">
+        <v>88</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="24" t="s">
-        <v>90</v>
-      </c>
-      <c r="E35" s="16" t="s">
-        <v>76</v>
-      </c>
-      <c r="F35" s="14" t="s">
+      <c r="D35" s="26" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="F35" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G35" s="1"/>
@@ -2387,24 +2408,24 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
-      <c r="S35" s="14" t="s">
+      <c r="S35" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
-      <c r="X35" s="14"/>
+      <c r="X35" s="16"/>
     </row>
     <row r="36" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="14"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="25"/>
-      <c r="E36" s="17"/>
-      <c r="F36" s="14" t="s">
+      <c r="D36" s="27"/>
+      <c r="E36" s="19"/>
+      <c r="F36" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G36" s="1"/>
@@ -2419,28 +2440,28 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
-      <c r="S36" s="14" t="s">
+      <c r="S36" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
-      <c r="X36" s="14"/>
+      <c r="X36" s="16"/>
     </row>
     <row r="37" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="14"/>
+      <c r="A37" s="16"/>
       <c r="B37" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="24" t="s">
-        <v>91</v>
-      </c>
-      <c r="E37" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="F37" s="14" t="s">
+      <c r="D37" s="26" t="s">
+        <v>90</v>
+      </c>
+      <c r="E37" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="F37" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G37" s="1"/>
@@ -2455,24 +2476,24 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
-      <c r="S37" s="14" t="s">
+      <c r="S37" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
-      <c r="X37" s="14"/>
+      <c r="X37" s="16"/>
     </row>
     <row r="38" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="14"/>
+      <c r="A38" s="16"/>
       <c r="B38" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="25"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="14" t="s">
+      <c r="D38" s="27"/>
+      <c r="E38" s="19"/>
+      <c r="F38" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G38" s="1"/>
@@ -2487,24 +2508,24 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
-      <c r="S38" s="14" t="s">
+      <c r="S38" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
-      <c r="X38" s="14"/>
+      <c r="X38" s="16"/>
     </row>
     <row r="39" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="14"/>
+      <c r="A39" s="16"/>
       <c r="B39" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G39" s="1"/>
@@ -2519,24 +2540,24 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
-      <c r="S39" s="14" t="s">
+      <c r="S39" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
-      <c r="X39" s="14"/>
+      <c r="X39" s="16"/>
     </row>
     <row r="40" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="14"/>
+      <c r="A40" s="16"/>
       <c r="B40" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="14" t="s">
+      <c r="F40" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G40" s="1"/>
@@ -2551,18 +2572,18 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
-      <c r="S40" s="14" t="s">
+      <c r="S40" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
-      <c r="X40" s="14"/>
+      <c r="X40" s="16"/>
     </row>
     <row r="41" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="14" t="s">
-        <v>92</v>
+      <c r="A41" s="16" t="s">
+        <v>91</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>50</v>
@@ -2570,7 +2591,7 @@
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="14" t="s">
+      <c r="F41" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G41" s="1"/>
@@ -2585,26 +2606,26 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
-      <c r="S41" s="14" t="s">
+      <c r="S41" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T41" s="1"/>
       <c r="U41" s="1"/>
       <c r="V41" s="1"/>
       <c r="W41" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="X41" s="14"/>
+        <v>92</v>
+      </c>
+      <c r="X41" s="16"/>
     </row>
     <row r="42" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="14"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="14" t="s">
+      <c r="F42" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G42" s="1"/>
@@ -2619,26 +2640,26 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
-      <c r="S42" s="14" t="s">
+      <c r="S42" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T42" s="1"/>
       <c r="U42" s="1"/>
       <c r="V42" s="1"/>
       <c r="W42" s="9" t="s">
-        <v>94</v>
-      </c>
-      <c r="X42" s="14"/>
+        <v>93</v>
+      </c>
+      <c r="X42" s="16"/>
     </row>
     <row r="43" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="14"/>
+      <c r="A43" s="16"/>
       <c r="B43" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="14" t="s">
+      <c r="F43" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G43" s="1"/>
@@ -2653,26 +2674,26 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
-      <c r="S43" s="14" t="s">
+      <c r="S43" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T43" s="1"/>
       <c r="U43" s="1"/>
       <c r="V43" s="1"/>
       <c r="W43" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="X43" s="14"/>
+        <v>94</v>
+      </c>
+      <c r="X43" s="16"/>
     </row>
     <row r="44" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="14"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="14" t="s">
+      <c r="F44" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G44" s="1"/>
@@ -2687,26 +2708,26 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
-      <c r="S44" s="14" t="s">
+      <c r="S44" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T44" s="1"/>
       <c r="U44" s="1"/>
       <c r="V44" s="1"/>
       <c r="W44" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="X44" s="14"/>
+        <v>95</v>
+      </c>
+      <c r="X44" s="16"/>
     </row>
     <row r="45" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="14"/>
+      <c r="A45" s="16"/>
       <c r="B45" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="14" t="s">
+      <c r="F45" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G45" s="1"/>
@@ -2721,26 +2742,26 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
-      <c r="S45" s="14" t="s">
+      <c r="S45" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T45" s="1"/>
       <c r="U45" s="1"/>
       <c r="V45" s="1"/>
       <c r="W45" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="X45" s="14"/>
+        <v>96</v>
+      </c>
+      <c r="X45" s="16"/>
     </row>
     <row r="46" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="14"/>
+      <c r="A46" s="16"/>
       <c r="B46" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="14" t="s">
+      <c r="F46" s="16" t="s">
         <v>3</v>
       </c>
       <c r="G46" s="1"/>
@@ -2755,42 +2776,42 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
-      <c r="S46" s="14" t="s">
+      <c r="S46" s="16" t="s">
         <v>3</v>
       </c>
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
-      <c r="X46" s="14"/>
+      <c r="X46" s="16"/>
     </row>
     <row r="47" spans="1:24" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="23" t="s">
-        <v>98</v>
-      </c>
-      <c r="B47" s="14"/>
-      <c r="C47" s="14"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="14"/>
-      <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="14"/>
-      <c r="I47" s="14"/>
-      <c r="J47" s="14"/>
-      <c r="K47" s="14"/>
-      <c r="L47" s="14"/>
-      <c r="M47" s="14"/>
-      <c r="N47" s="14"/>
-      <c r="O47" s="14"/>
-      <c r="P47" s="14"/>
-      <c r="Q47" s="14"/>
-      <c r="R47" s="14"/>
-      <c r="S47" s="14"/>
-      <c r="T47" s="14"/>
-      <c r="U47" s="14"/>
-      <c r="V47" s="14"/>
-      <c r="W47" s="14"/>
-      <c r="X47" s="14"/>
+      <c r="A47" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="16"/>
+      <c r="C47" s="16"/>
+      <c r="D47" s="16"/>
+      <c r="E47" s="16"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="16"/>
+      <c r="H47" s="16"/>
+      <c r="I47" s="16"/>
+      <c r="J47" s="16"/>
+      <c r="K47" s="16"/>
+      <c r="L47" s="16"/>
+      <c r="M47" s="16"/>
+      <c r="N47" s="16"/>
+      <c r="O47" s="16"/>
+      <c r="P47" s="16"/>
+      <c r="Q47" s="16"/>
+      <c r="R47" s="16"/>
+      <c r="S47" s="16"/>
+      <c r="T47" s="16"/>
+      <c r="U47" s="16"/>
+      <c r="V47" s="16"/>
+      <c r="W47" s="16"/>
+      <c r="X47" s="16"/>
     </row>
   </sheetData>
   <mergeCells count="29">
@@ -2819,12 +2840,12 @@
     <mergeCell ref="S29:S46"/>
     <mergeCell ref="X5:X46"/>
     <mergeCell ref="I21:I22"/>
-    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="L15:L16"/>
     <mergeCell ref="K21:K22"/>
-    <mergeCell ref="N9:N10"/>
+    <mergeCell ref="M26:M27"/>
     <mergeCell ref="N21:N22"/>
   </mergeCells>
-  <phoneticPr fontId="8" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="8" orientation="landscape" horizontalDpi="300" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>

</xml_diff>

<commit_message>
Modified my schedule and initialed next semester schedule.
</commit_message>
<xml_diff>
--- a/2020-2021 1st semester schedule.xlsx
+++ b/2020-2021 1st semester schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20369"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Baron_Red\Desktop\MySchedule\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\MySchedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66D01403-764B-45FD-9577-5F8DF84E72E9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCBF727-BE17-4180-B2C3-6026667A3B0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="107">
   <si>
     <t>刘锐教师课表</t>
   </si>
@@ -337,6 +337,14 @@
   </si>
   <si>
     <t>计算机网络1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX3</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX4</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -360,15 +368,8 @@
 TX2--信息18-2
 计算机网络1--信息18
 TX3--电气18-5
-TX4--电气18-6</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>TX3</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <t>TX4</t>
+TX4--电气18-6
+PYTHON--信息18</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -553,7 +554,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -603,13 +604,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -640,9 +641,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -923,24 +921,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="U24" sqref="U24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
     <col min="2" max="2" width="6" customWidth="1"/>
     <col min="3" max="12" width="6" hidden="1" customWidth="1"/>
     <col min="13" max="15" width="6" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="11.06640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11" bestFit="1" customWidth="1"/>
     <col min="19" max="22" width="6" customWidth="1"/>
-    <col min="23" max="23" width="20.3984375" customWidth="1"/>
+    <col min="23" max="23" width="20.42578125" customWidth="1"/>
     <col min="24" max="24" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:24" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24" t="s">
         <v>0</v>
       </c>
@@ -968,7 +966,7 @@
       <c r="W1" s="20"/>
       <c r="X1" s="20"/>
     </row>
-    <row r="2" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
@@ -998,7 +996,7 @@
       <c r="W2" s="20"/>
       <c r="X2" s="20"/>
     </row>
-    <row r="3" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -1072,7 +1070,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>27</v>
       </c>
@@ -1146,7 +1144,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="20" t="s">
         <v>49</v>
       </c>
@@ -1193,7 +1191,9 @@
       <c r="R5" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="S5" s="1"/>
+      <c r="S5" s="19" t="s">
+        <v>105</v>
+      </c>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
@@ -1201,10 +1201,10 @@
         <v>54</v>
       </c>
       <c r="X5" s="21" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="20"/>
       <c r="B6" s="1" t="s">
         <v>55</v>
@@ -1240,7 +1240,7 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-      <c r="P6" s="18"/>
+      <c r="P6" s="17"/>
       <c r="Q6" s="13" t="s">
         <v>103</v>
       </c>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="X6" s="20"/>
     </row>
-    <row r="7" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20"/>
       <c r="B7" s="1" t="s">
         <v>58</v>
@@ -1282,7 +1282,7 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-      <c r="P7" s="18"/>
+      <c r="P7" s="17"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
@@ -1292,7 +1292,7 @@
       <c r="W7" s="1"/>
       <c r="X7" s="20"/>
     </row>
-    <row r="8" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="20"/>
       <c r="B8" s="1" t="s">
         <v>59</v>
@@ -1314,7 +1314,7 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-      <c r="P8" s="18"/>
+      <c r="P8" s="17"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
@@ -1324,7 +1324,7 @@
       <c r="W8" s="1"/>
       <c r="X8" s="20"/>
     </row>
-    <row r="9" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20"/>
       <c r="B9" s="1" t="s">
         <v>60</v>
@@ -1360,7 +1360,7 @@
       </c>
       <c r="X9" s="20"/>
     </row>
-    <row r="10" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20"/>
       <c r="B10" s="1" t="s">
         <v>64</v>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="X10" s="20"/>
     </row>
-    <row r="11" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
         <v>66</v>
       </c>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="X11" s="20"/>
     </row>
-    <row r="12" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20"/>
       <c r="B12" s="1" t="s">
         <v>55</v>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="X12" s="20"/>
     </row>
-    <row r="13" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20"/>
       <c r="B13" s="1" t="s">
         <v>58</v>
@@ -1548,7 +1548,7 @@
       </c>
       <c r="X13" s="20"/>
     </row>
-    <row r="14" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20"/>
       <c r="B14" s="1" t="s">
         <v>59</v>
@@ -1600,7 +1600,7 @@
       </c>
       <c r="X14" s="20"/>
     </row>
-    <row r="15" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20"/>
       <c r="B15" s="1" t="s">
         <v>60</v>
@@ -1632,7 +1632,7 @@
       <c r="W15" s="1"/>
       <c r="X15" s="20"/>
     </row>
-    <row r="16" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
       <c r="B16" s="1" t="s">
         <v>64</v>
@@ -1662,7 +1662,7 @@
       <c r="W16" s="1"/>
       <c r="X16" s="20"/>
     </row>
-    <row r="17" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
         <v>73</v>
       </c>
@@ -1686,7 +1686,7 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1"/>
-      <c r="R17" s="19"/>
+      <c r="R17" s="18"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
@@ -1694,7 +1694,7 @@
       <c r="W17" s="1"/>
       <c r="X17" s="20"/>
     </row>
-    <row r="18" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
       <c r="B18" s="1" t="s">
         <v>55</v>
@@ -1732,7 +1732,7 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1"/>
-      <c r="R18" s="19"/>
+      <c r="R18" s="18"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
@@ -1742,7 +1742,7 @@
       </c>
       <c r="X18" s="20"/>
     </row>
-    <row r="19" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="1" t="s">
         <v>58</v>
@@ -1794,7 +1794,7 @@
       </c>
       <c r="X19" s="20"/>
     </row>
-    <row r="20" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20"/>
       <c r="B20" s="1" t="s">
         <v>59</v>
@@ -1828,7 +1828,7 @@
       <c r="W20" s="1"/>
       <c r="X20" s="20"/>
     </row>
-    <row r="21" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20"/>
       <c r="B21" s="1" t="s">
         <v>60</v>
@@ -1862,7 +1862,7 @@
       <c r="Q21" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="R21" s="17" t="s">
+      <c r="R21" s="13" t="s">
         <v>103</v>
       </c>
       <c r="S21" s="1"/>
@@ -1874,7 +1874,7 @@
       </c>
       <c r="X21" s="20"/>
     </row>
-    <row r="22" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20"/>
       <c r="B22" s="1" t="s">
         <v>64</v>
@@ -1900,7 +1900,7 @@
       <c r="Q22" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="R22" s="17" t="s">
+      <c r="R22" s="13" t="s">
         <v>103</v>
       </c>
       <c r="S22" s="1"/>
@@ -1912,7 +1912,7 @@
       </c>
       <c r="X22" s="20"/>
     </row>
-    <row r="23" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
         <v>78</v>
       </c>
@@ -1950,7 +1950,7 @@
       <c r="W23" s="1"/>
       <c r="X23" s="20"/>
     </row>
-    <row r="24" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20"/>
       <c r="B24" s="1" t="s">
         <v>55</v>
@@ -1988,7 +1988,7 @@
       <c r="Q24" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="R24" s="5" t="s">
+      <c r="R24" s="4" t="s">
         <v>52</v>
       </c>
       <c r="S24" s="5" t="s">
@@ -2004,7 +2004,7 @@
       </c>
       <c r="X24" s="20"/>
     </row>
-    <row r="25" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20"/>
       <c r="B25" s="1" t="s">
         <v>58</v>
@@ -2056,7 +2056,7 @@
       </c>
       <c r="X25" s="20"/>
     </row>
-    <row r="26" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20"/>
       <c r="B26" s="1" t="s">
         <v>59</v>
@@ -2112,7 +2112,7 @@
       </c>
       <c r="X26" s="20"/>
     </row>
-    <row r="27" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20"/>
       <c r="B27" s="1" t="s">
         <v>60</v>
@@ -2154,7 +2154,7 @@
       </c>
       <c r="X27" s="20"/>
     </row>
-    <row r="28" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20"/>
       <c r="B28" s="1" t="s">
         <v>64</v>
@@ -2192,7 +2192,7 @@
       </c>
       <c r="X28" s="20"/>
     </row>
-    <row r="29" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
         <v>84</v>
       </c>
@@ -2226,7 +2226,7 @@
       <c r="Q29" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="R29" s="5" t="s">
+      <c r="R29" s="4" t="s">
         <v>52</v>
       </c>
       <c r="S29" s="20" t="s">
@@ -2240,7 +2240,7 @@
       </c>
       <c r="X29" s="20"/>
     </row>
-    <row r="30" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20"/>
       <c r="B30" s="1" t="s">
         <v>55</v>
@@ -2278,8 +2278,8 @@
       <c r="O30" s="1"/>
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
-      <c r="R30" s="30" t="s">
-        <v>105</v>
+      <c r="R30" s="4" t="s">
+        <v>104</v>
       </c>
       <c r="S30" s="20" t="s">
         <v>3</v>
@@ -2292,7 +2292,7 @@
       </c>
       <c r="X30" s="20"/>
     </row>
-    <row r="31" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="20"/>
       <c r="B31" s="1" t="s">
         <v>58</v>
@@ -2314,10 +2314,7 @@
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
       <c r="Q31" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="R31" s="30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="S31" s="20" t="s">
         <v>3</v>
@@ -2328,7 +2325,7 @@
       <c r="W31" s="1"/>
       <c r="X31" s="20"/>
     </row>
-    <row r="32" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="20"/>
       <c r="B32" s="1" t="s">
         <v>59</v>
@@ -2354,7 +2351,7 @@
       <c r="O32" s="6"/>
       <c r="P32" s="6"/>
       <c r="Q32" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="R32" s="1"/>
       <c r="S32" s="20" t="s">
@@ -2368,7 +2365,7 @@
       </c>
       <c r="X32" s="20"/>
     </row>
-    <row r="33" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="20"/>
       <c r="B33" s="1" t="s">
         <v>60</v>
@@ -2402,7 +2399,7 @@
       <c r="W33" s="1"/>
       <c r="X33" s="20"/>
     </row>
-    <row r="34" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="20"/>
       <c r="B34" s="1" t="s">
         <v>64</v>
@@ -2436,7 +2433,7 @@
       <c r="W34" s="1"/>
       <c r="X34" s="20"/>
     </row>
-    <row r="35" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
         <v>88</v>
       </c>
@@ -2474,7 +2471,7 @@
       <c r="W35" s="1"/>
       <c r="X35" s="20"/>
     </row>
-    <row r="36" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="20"/>
       <c r="B36" s="1" t="s">
         <v>55</v>
@@ -2506,7 +2503,7 @@
       <c r="W36" s="1"/>
       <c r="X36" s="20"/>
     </row>
-    <row r="37" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="20"/>
       <c r="B37" s="1" t="s">
         <v>58</v>
@@ -2542,7 +2539,7 @@
       <c r="W37" s="1"/>
       <c r="X37" s="20"/>
     </row>
-    <row r="38" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="20"/>
       <c r="B38" s="1" t="s">
         <v>59</v>
@@ -2574,7 +2571,7 @@
       <c r="W38" s="1"/>
       <c r="X38" s="20"/>
     </row>
-    <row r="39" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20"/>
       <c r="B39" s="1" t="s">
         <v>60</v>
@@ -2606,7 +2603,7 @@
       <c r="W39" s="1"/>
       <c r="X39" s="20"/>
     </row>
-    <row r="40" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="20"/>
       <c r="B40" s="1" t="s">
         <v>64</v>
@@ -2638,7 +2635,7 @@
       <c r="W40" s="1"/>
       <c r="X40" s="20"/>
     </row>
-    <row r="41" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
         <v>91</v>
       </c>
@@ -2674,7 +2671,7 @@
       </c>
       <c r="X41" s="20"/>
     </row>
-    <row r="42" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="20"/>
       <c r="B42" s="1" t="s">
         <v>55</v>
@@ -2708,7 +2705,7 @@
       </c>
       <c r="X42" s="20"/>
     </row>
-    <row r="43" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="20"/>
       <c r="B43" s="1" t="s">
         <v>58</v>
@@ -2742,7 +2739,7 @@
       </c>
       <c r="X43" s="20"/>
     </row>
-    <row r="44" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="20"/>
       <c r="B44" s="1" t="s">
         <v>59</v>
@@ -2776,7 +2773,7 @@
       </c>
       <c r="X44" s="20"/>
     </row>
-    <row r="45" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="20"/>
       <c r="B45" s="1" t="s">
         <v>60</v>
@@ -2810,7 +2807,7 @@
       </c>
       <c r="X45" s="20"/>
     </row>
-    <row r="46" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="20"/>
       <c r="B46" s="1" t="s">
         <v>64</v>
@@ -2842,7 +2839,7 @@
       <c r="W46" s="1"/>
       <c r="X46" s="20"/>
     </row>
-    <row r="47" spans="1:24" ht="32.1" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:24" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="27" t="s">
         <v>97</v>
       </c>

</xml_diff>

<commit_message>
Changed lots of files.
</commit_message>
<xml_diff>
--- a/2020-2021 1st semester schedule.xlsx
+++ b/2020-2021 1st semester schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\MySchedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCBF727-BE17-4180-B2C3-6026667A3B0F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1D3779B-F13F-4BED-A1BD-4E4E994E0693}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="108">
   <si>
     <t>刘锐教师课表</t>
   </si>
@@ -370,6 +370,10 @@
 TX3--电气18-5
 TX4--电气18-6
 PYTHON--信息18</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>PYTHON</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -610,9 +614,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -641,6 +642,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -922,7 +926,7 @@
   <dimension ref="A1:X47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W21" sqref="W21"/>
+      <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -933,68 +937,69 @@
     <col min="13" max="15" width="6" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
     <col min="17" max="18" width="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="22" width="6" customWidth="1"/>
+    <col min="19" max="19" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="6" customWidth="1"/>
     <col min="23" max="23" width="20.42578125" customWidth="1"/>
     <col min="24" max="24" width="27" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="20"/>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
     </row>
     <row r="2" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="26" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+      <c r="V2" s="19"/>
+      <c r="W2" s="19"/>
+      <c r="X2" s="19"/>
     </row>
     <row r="3" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1145,7 +1150,7 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="19" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
@@ -1163,7 +1168,7 @@
       <c r="F5" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="19" t="s">
         <v>53</v>
       </c>
       <c r="H5" s="4" t="s">
@@ -1191,7 +1196,7 @@
       <c r="R5" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="S5" s="19" t="s">
+      <c r="S5" s="4" t="s">
         <v>105</v>
       </c>
       <c r="T5" s="1"/>
@@ -1200,12 +1205,12 @@
       <c r="W5" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="X5" s="21" t="s">
+      <c r="X5" s="20" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20"/>
+      <c r="A6" s="19"/>
       <c r="B6" s="1" t="s">
         <v>55</v>
       </c>
@@ -1221,7 +1226,7 @@
       <c r="F6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="20" t="s">
+      <c r="G6" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="4" t="s">
@@ -1254,10 +1259,10 @@
       <c r="W6" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="X6" s="20"/>
+      <c r="X6" s="19"/>
     </row>
     <row r="7" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="20"/>
+      <c r="A7" s="19"/>
       <c r="B7" s="1" t="s">
         <v>58</v>
       </c>
@@ -1267,7 +1272,7 @@
       <c r="F7" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="G7" s="20" t="s">
+      <c r="G7" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H7" s="1"/>
@@ -1290,10 +1295,10 @@
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
       <c r="W7" s="1"/>
-      <c r="X7" s="20"/>
+      <c r="X7" s="19"/>
     </row>
     <row r="8" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="20"/>
+      <c r="A8" s="19"/>
       <c r="B8" s="1" t="s">
         <v>59</v>
       </c>
@@ -1303,7 +1308,7 @@
       <c r="F8" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="G8" s="20" t="s">
+      <c r="G8" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H8" s="1"/>
@@ -1322,10 +1327,10 @@
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
       <c r="W8" s="1"/>
-      <c r="X8" s="20"/>
+      <c r="X8" s="19"/>
     </row>
     <row r="9" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
+      <c r="A9" s="19"/>
       <c r="B9" s="1" t="s">
         <v>60</v>
       </c>
@@ -1333,7 +1338,7 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="20" t="s">
+      <c r="G9" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H9" s="6"/>
@@ -1358,10 +1363,10 @@
       <c r="W9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="X9" s="20"/>
+      <c r="X9" s="19"/>
     </row>
     <row r="10" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="20"/>
+      <c r="A10" s="19"/>
       <c r="B10" s="1" t="s">
         <v>64</v>
       </c>
@@ -1369,7 +1374,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H10" s="1"/>
@@ -1394,10 +1399,10 @@
       <c r="W10" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="X10" s="20"/>
+      <c r="X10" s="19"/>
     </row>
     <row r="11" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="20" t="s">
+      <c r="A11" s="19" t="s">
         <v>66</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1407,7 +1412,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H11" s="1"/>
@@ -1434,10 +1439,10 @@
       <c r="W11" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="X11" s="20"/>
+      <c r="X11" s="19"/>
     </row>
     <row r="12" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="20"/>
+      <c r="A12" s="19"/>
       <c r="B12" s="1" t="s">
         <v>55</v>
       </c>
@@ -1445,7 +1450,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
-      <c r="G12" s="20" t="s">
+      <c r="G12" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H12" s="1"/>
@@ -1484,10 +1489,10 @@
       <c r="W12" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="X12" s="20"/>
+      <c r="X12" s="19"/>
     </row>
     <row r="13" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="20"/>
+      <c r="A13" s="19"/>
       <c r="B13" s="1" t="s">
         <v>58</v>
       </c>
@@ -1503,7 +1508,7 @@
       <c r="F13" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G13" s="20" t="s">
+      <c r="G13" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H13" s="4" t="s">
@@ -1546,10 +1551,10 @@
       <c r="W13" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="X13" s="20"/>
+      <c r="X13" s="19"/>
     </row>
     <row r="14" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="20"/>
+      <c r="A14" s="19"/>
       <c r="B14" s="1" t="s">
         <v>59</v>
       </c>
@@ -1565,7 +1570,7 @@
       <c r="F14" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H14" s="4" t="s">
@@ -1598,10 +1603,10 @@
       <c r="W14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="X14" s="20"/>
+      <c r="X14" s="19"/>
     </row>
     <row r="15" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="20"/>
+      <c r="A15" s="19"/>
       <c r="B15" s="1" t="s">
         <v>60</v>
       </c>
@@ -1609,14 +1614,14 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="14"/>
-      <c r="L15" s="22" t="s">
+      <c r="L15" s="21" t="s">
         <v>61</v>
       </c>
       <c r="M15" s="1"/>
@@ -1630,10 +1635,10 @@
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
       <c r="W15" s="1"/>
-      <c r="X15" s="20"/>
+      <c r="X15" s="19"/>
     </row>
     <row r="16" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="20"/>
+      <c r="A16" s="19"/>
       <c r="B16" s="1" t="s">
         <v>64</v>
       </c>
@@ -1641,14 +1646,14 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
-      <c r="G16" s="20" t="s">
+      <c r="G16" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="14"/>
-      <c r="L16" s="23"/>
+      <c r="L16" s="22"/>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
@@ -1660,10 +1665,10 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
       <c r="W16" s="1"/>
-      <c r="X16" s="20"/>
+      <c r="X16" s="19"/>
     </row>
     <row r="17" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="20" t="s">
+      <c r="A17" s="19" t="s">
         <v>73</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1673,7 +1678,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
-      <c r="G17" s="20" t="s">
+      <c r="G17" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H17" s="1"/>
@@ -1692,10 +1697,10 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
       <c r="W17" s="1"/>
-      <c r="X17" s="20"/>
+      <c r="X17" s="19"/>
     </row>
     <row r="18" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="20"/>
+      <c r="A18" s="19"/>
       <c r="B18" s="1" t="s">
         <v>55</v>
       </c>
@@ -1711,7 +1716,7 @@
       <c r="F18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G18" s="20" t="s">
+      <c r="G18" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H18" s="4" t="s">
@@ -1740,10 +1745,10 @@
       <c r="W18" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="X18" s="20"/>
+      <c r="X18" s="19"/>
     </row>
     <row r="19" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="20"/>
+      <c r="A19" s="19"/>
       <c r="B19" s="1" t="s">
         <v>58</v>
       </c>
@@ -1759,7 +1764,7 @@
       <c r="F19" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="20" t="s">
+      <c r="G19" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H19" s="4" t="s">
@@ -1792,10 +1797,10 @@
       <c r="W19" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="X19" s="20"/>
+      <c r="X19" s="19"/>
     </row>
     <row r="20" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="20"/>
+      <c r="A20" s="19"/>
       <c r="B20" s="1" t="s">
         <v>59</v>
       </c>
@@ -1805,7 +1810,7 @@
         <v>98</v>
       </c>
       <c r="F20" s="1"/>
-      <c r="G20" s="20" t="s">
+      <c r="G20" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H20" s="1"/>
@@ -1826,10 +1831,10 @@
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
       <c r="W20" s="1"/>
-      <c r="X20" s="20"/>
+      <c r="X20" s="19"/>
     </row>
     <row r="21" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
+      <c r="A21" s="19"/>
       <c r="B21" s="1" t="s">
         <v>60</v>
       </c>
@@ -1837,22 +1842,22 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
-      <c r="G21" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="H21" s="22" t="s">
+      <c r="G21" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="I21" s="22" t="s">
+      <c r="I21" s="21" t="s">
         <v>76</v>
       </c>
       <c r="J21" s="7"/>
-      <c r="K21" s="22" t="s">
+      <c r="K21" s="21" t="s">
         <v>77</v>
       </c>
       <c r="L21" s="1"/>
       <c r="M21" s="1"/>
-      <c r="N21" s="22" t="s">
+      <c r="N21" s="21" t="s">
         <v>77</v>
       </c>
       <c r="O21" s="1"/>
@@ -1865,17 +1870,19 @@
       <c r="R21" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="S21" s="1"/>
+      <c r="S21" s="29" t="s">
+        <v>107</v>
+      </c>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
       <c r="W21" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="X21" s="20"/>
+      <c r="X21" s="19"/>
     </row>
     <row r="22" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
+      <c r="A22" s="19"/>
       <c r="B22" s="1" t="s">
         <v>64</v>
       </c>
@@ -1883,16 +1890,16 @@
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-      <c r="G22" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="H22" s="23"/>
-      <c r="I22" s="23"/>
+      <c r="G22" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="22"/>
+      <c r="I22" s="22"/>
       <c r="J22" s="7"/>
-      <c r="K22" s="23"/>
+      <c r="K22" s="22"/>
       <c r="L22" s="1"/>
       <c r="M22" s="1"/>
-      <c r="N22" s="23"/>
+      <c r="N22" s="22"/>
       <c r="O22" s="1"/>
       <c r="P22" s="4" t="s">
         <v>65</v>
@@ -1903,17 +1910,19 @@
       <c r="R22" s="13" t="s">
         <v>103</v>
       </c>
-      <c r="S22" s="1"/>
+      <c r="S22" s="29" t="s">
+        <v>107</v>
+      </c>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
       <c r="W22" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="X22" s="20"/>
+      <c r="X22" s="19"/>
     </row>
     <row r="23" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="20" t="s">
+      <c r="A23" s="19" t="s">
         <v>78</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -1921,16 +1930,16 @@
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="G23" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="H23" s="22" t="s">
+      <c r="G23" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H23" s="21" t="s">
         <v>79</v>
       </c>
       <c r="I23" s="1"/>
@@ -1948,23 +1957,23 @@
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
       <c r="W23" s="1"/>
-      <c r="X23" s="20"/>
+      <c r="X23" s="19"/>
     </row>
     <row r="24" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20"/>
+      <c r="A24" s="19"/>
       <c r="B24" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="G24" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="H24" s="23"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G24" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H24" s="22"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="13" t="s">
@@ -2002,10 +2011,10 @@
       <c r="W24" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="X24" s="20"/>
+      <c r="X24" s="19"/>
     </row>
     <row r="25" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="20"/>
+      <c r="A25" s="19"/>
       <c r="B25" s="1" t="s">
         <v>58</v>
       </c>
@@ -2018,10 +2027,10 @@
       <c r="E25" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F25" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" s="20" t="s">
+      <c r="F25" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G25" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H25" s="4" t="s">
@@ -2054,10 +2063,10 @@
       <c r="W25" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="X25" s="20"/>
+      <c r="X25" s="19"/>
     </row>
     <row r="26" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
+      <c r="A26" s="19"/>
       <c r="B26" s="1" t="s">
         <v>59</v>
       </c>
@@ -2070,10 +2079,10 @@
       <c r="E26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F26" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="G26" s="20" t="s">
+      <c r="F26" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="19" t="s">
         <v>3</v>
       </c>
       <c r="H26" s="4" t="s">
@@ -2091,7 +2100,7 @@
       <c r="L26" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="M26" s="22" t="s">
+      <c r="M26" s="21" t="s">
         <v>61</v>
       </c>
       <c r="N26" s="1"/>
@@ -2110,32 +2119,32 @@
       <c r="W26" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="X26" s="20"/>
+      <c r="X26" s="19"/>
     </row>
     <row r="27" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="20"/>
+      <c r="A27" s="19"/>
       <c r="B27" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
-      <c r="E27" s="22" t="s">
+      <c r="E27" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="F27" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="G27" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="H27" s="22" t="s">
+      <c r="F27" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="21" t="s">
         <v>83</v>
       </c>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-      <c r="M27" s="23"/>
+      <c r="M27" s="22"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="4" t="s">
@@ -2152,23 +2161,23 @@
       <c r="W27" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="X27" s="20"/>
+      <c r="X27" s="19"/>
     </row>
     <row r="28" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="20"/>
+      <c r="A28" s="19"/>
       <c r="B28" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="G28" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="H28" s="23"/>
+      <c r="E28" s="22"/>
+      <c r="F28" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="H28" s="22"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
@@ -2190,10 +2199,10 @@
       <c r="W28" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="X28" s="20"/>
+      <c r="X28" s="19"/>
     </row>
     <row r="29" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="19" t="s">
         <v>84</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2202,7 +2211,7 @@
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G29" s="1"/>
@@ -2229,7 +2238,7 @@
       <c r="R29" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="S29" s="20" t="s">
+      <c r="S29" s="19" t="s">
         <v>85</v>
       </c>
       <c r="T29" s="1"/>
@@ -2238,10 +2247,10 @@
       <c r="W29" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="X29" s="20"/>
+      <c r="X29" s="19"/>
     </row>
     <row r="30" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="20"/>
+      <c r="A30" s="19"/>
       <c r="B30" s="1" t="s">
         <v>55</v>
       </c>
@@ -2254,7 +2263,7 @@
       <c r="E30" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F30" s="20" t="s">
+      <c r="F30" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G30" s="4" t="s">
@@ -2281,7 +2290,7 @@
       <c r="R30" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="S30" s="20" t="s">
+      <c r="S30" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T30" s="1"/>
@@ -2290,17 +2299,17 @@
       <c r="W30" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="X30" s="20"/>
+      <c r="X30" s="19"/>
     </row>
     <row r="31" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="20"/>
+      <c r="A31" s="19"/>
       <c r="B31" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="20" t="s">
+      <c r="F31" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G31" s="1"/>
@@ -2316,24 +2325,24 @@
       <c r="Q31" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="S31" s="20" t="s">
+      <c r="S31" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
       <c r="W31" s="1"/>
-      <c r="X31" s="20"/>
+      <c r="X31" s="19"/>
     </row>
     <row r="32" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="20"/>
+      <c r="A32" s="19"/>
       <c r="B32" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="20" t="s">
+      <c r="F32" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G32" s="1"/>
@@ -2354,7 +2363,7 @@
         <v>105</v>
       </c>
       <c r="R32" s="1"/>
-      <c r="S32" s="20" t="s">
+      <c r="S32" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T32" s="1"/>
@@ -2363,17 +2372,17 @@
       <c r="W32" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="X32" s="20"/>
+      <c r="X32" s="19"/>
     </row>
     <row r="33" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="20"/>
+      <c r="A33" s="19"/>
       <c r="B33" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-      <c r="F33" s="20" t="s">
+      <c r="F33" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G33" s="1"/>
@@ -2390,24 +2399,24 @@
         <v>103</v>
       </c>
       <c r="R33" s="1"/>
-      <c r="S33" s="20" t="s">
+      <c r="S33" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T33" s="1"/>
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
-      <c r="X33" s="20"/>
+      <c r="X33" s="19"/>
     </row>
     <row r="34" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="20"/>
+      <c r="A34" s="19"/>
       <c r="B34" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="20" t="s">
+      <c r="F34" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G34" s="1"/>
@@ -2424,30 +2433,30 @@
         <v>103</v>
       </c>
       <c r="R34" s="1"/>
-      <c r="S34" s="20" t="s">
+      <c r="S34" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T34" s="1"/>
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
-      <c r="X34" s="20"/>
+      <c r="X34" s="19"/>
     </row>
     <row r="35" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="19" t="s">
         <v>88</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>50</v>
       </c>
       <c r="C35" s="1"/>
-      <c r="D35" s="28" t="s">
+      <c r="D35" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="E35" s="22" t="s">
+      <c r="E35" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="F35" s="20" t="s">
+      <c r="F35" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G35" s="1"/>
@@ -2462,24 +2471,24 @@
       <c r="P35" s="1"/>
       <c r="Q35" s="1"/>
       <c r="R35" s="1"/>
-      <c r="S35" s="20" t="s">
+      <c r="S35" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
-      <c r="X35" s="20"/>
+      <c r="X35" s="19"/>
     </row>
     <row r="36" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="20"/>
+      <c r="A36" s="19"/>
       <c r="B36" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C36" s="1"/>
-      <c r="D36" s="29"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="20" t="s">
+      <c r="D36" s="28"/>
+      <c r="E36" s="22"/>
+      <c r="F36" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G36" s="1"/>
@@ -2494,28 +2503,28 @@
       <c r="P36" s="1"/>
       <c r="Q36" s="1"/>
       <c r="R36" s="1"/>
-      <c r="S36" s="20" t="s">
+      <c r="S36" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
-      <c r="X36" s="20"/>
+      <c r="X36" s="19"/>
     </row>
     <row r="37" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="20"/>
+      <c r="A37" s="19"/>
       <c r="B37" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C37" s="1"/>
-      <c r="D37" s="28" t="s">
+      <c r="D37" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E37" s="22" t="s">
+      <c r="E37" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="F37" s="20" t="s">
+      <c r="F37" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G37" s="1"/>
@@ -2530,24 +2539,24 @@
       <c r="P37" s="1"/>
       <c r="Q37" s="1"/>
       <c r="R37" s="1"/>
-      <c r="S37" s="20" t="s">
+      <c r="S37" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T37" s="1"/>
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
-      <c r="X37" s="20"/>
+      <c r="X37" s="19"/>
     </row>
     <row r="38" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="20"/>
+      <c r="A38" s="19"/>
       <c r="B38" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C38" s="1"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="20" t="s">
+      <c r="D38" s="28"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G38" s="1"/>
@@ -2562,24 +2571,24 @@
       <c r="P38" s="1"/>
       <c r="Q38" s="1"/>
       <c r="R38" s="1"/>
-      <c r="S38" s="20" t="s">
+      <c r="S38" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T38" s="1"/>
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
-      <c r="X38" s="20"/>
+      <c r="X38" s="19"/>
     </row>
     <row r="39" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="20"/>
+      <c r="A39" s="19"/>
       <c r="B39" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-      <c r="F39" s="20" t="s">
+      <c r="F39" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G39" s="1"/>
@@ -2594,24 +2603,24 @@
       <c r="P39" s="1"/>
       <c r="Q39" s="1"/>
       <c r="R39" s="1"/>
-      <c r="S39" s="20" t="s">
+      <c r="S39" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T39" s="1"/>
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
-      <c r="X39" s="20"/>
+      <c r="X39" s="19"/>
     </row>
     <row r="40" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="20"/>
+      <c r="A40" s="19"/>
       <c r="B40" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="20" t="s">
+      <c r="F40" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G40" s="1"/>
@@ -2626,17 +2635,17 @@
       <c r="P40" s="1"/>
       <c r="Q40" s="1"/>
       <c r="R40" s="1"/>
-      <c r="S40" s="20" t="s">
+      <c r="S40" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T40" s="1"/>
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
-      <c r="X40" s="20"/>
+      <c r="X40" s="19"/>
     </row>
     <row r="41" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="20" t="s">
+      <c r="A41" s="19" t="s">
         <v>91</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -2645,7 +2654,7 @@
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="20" t="s">
+      <c r="F41" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G41" s="1"/>
@@ -2660,7 +2669,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
-      <c r="S41" s="20" t="s">
+      <c r="S41" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T41" s="1"/>
@@ -2669,17 +2678,17 @@
       <c r="W41" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="X41" s="20"/>
+      <c r="X41" s="19"/>
     </row>
     <row r="42" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="20"/>
+      <c r="A42" s="19"/>
       <c r="B42" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
-      <c r="F42" s="20" t="s">
+      <c r="F42" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G42" s="1"/>
@@ -2694,7 +2703,7 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
-      <c r="S42" s="20" t="s">
+      <c r="S42" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T42" s="1"/>
@@ -2703,17 +2712,17 @@
       <c r="W42" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="X42" s="20"/>
+      <c r="X42" s="19"/>
     </row>
     <row r="43" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="20"/>
+      <c r="A43" s="19"/>
       <c r="B43" s="1" t="s">
         <v>58</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="20" t="s">
+      <c r="F43" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G43" s="1"/>
@@ -2728,7 +2737,7 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
-      <c r="S43" s="20" t="s">
+      <c r="S43" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T43" s="1"/>
@@ -2737,17 +2746,17 @@
       <c r="W43" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="X43" s="20"/>
+      <c r="X43" s="19"/>
     </row>
     <row r="44" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="20"/>
+      <c r="A44" s="19"/>
       <c r="B44" s="1" t="s">
         <v>59</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="20" t="s">
+      <c r="F44" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G44" s="1"/>
@@ -2762,7 +2771,7 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
-      <c r="S44" s="20" t="s">
+      <c r="S44" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T44" s="1"/>
@@ -2771,17 +2780,17 @@
       <c r="W44" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="X44" s="20"/>
+      <c r="X44" s="19"/>
     </row>
     <row r="45" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="20"/>
+      <c r="A45" s="19"/>
       <c r="B45" s="1" t="s">
         <v>60</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
-      <c r="F45" s="20" t="s">
+      <c r="F45" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G45" s="1"/>
@@ -2796,7 +2805,7 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
-      <c r="S45" s="20" t="s">
+      <c r="S45" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T45" s="1"/>
@@ -2805,17 +2814,17 @@
       <c r="W45" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="X45" s="20"/>
+      <c r="X45" s="19"/>
     </row>
     <row r="46" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="20"/>
+      <c r="A46" s="19"/>
       <c r="B46" s="1" t="s">
         <v>64</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="20" t="s">
+      <c r="F46" s="19" t="s">
         <v>3</v>
       </c>
       <c r="G46" s="1"/>
@@ -2830,42 +2839,42 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
-      <c r="S46" s="20" t="s">
+      <c r="S46" s="19" t="s">
         <v>3</v>
       </c>
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
-      <c r="X46" s="20"/>
+      <c r="X46" s="19"/>
     </row>
     <row r="47" spans="1:24" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="27" t="s">
+      <c r="A47" s="26" t="s">
         <v>97</v>
       </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
-      <c r="K47" s="20"/>
-      <c r="L47" s="20"/>
-      <c r="M47" s="20"/>
-      <c r="N47" s="20"/>
-      <c r="O47" s="20"/>
-      <c r="P47" s="20"/>
-      <c r="Q47" s="20"/>
-      <c r="R47" s="20"/>
-      <c r="S47" s="20"/>
-      <c r="T47" s="20"/>
-      <c r="U47" s="20"/>
-      <c r="V47" s="20"/>
-      <c r="W47" s="20"/>
-      <c r="X47" s="20"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="19"/>
+      <c r="G47" s="19"/>
+      <c r="H47" s="19"/>
+      <c r="I47" s="19"/>
+      <c r="J47" s="19"/>
+      <c r="K47" s="19"/>
+      <c r="L47" s="19"/>
+      <c r="M47" s="19"/>
+      <c r="N47" s="19"/>
+      <c r="O47" s="19"/>
+      <c r="P47" s="19"/>
+      <c r="Q47" s="19"/>
+      <c r="R47" s="19"/>
+      <c r="S47" s="19"/>
+      <c r="T47" s="19"/>
+      <c r="U47" s="19"/>
+      <c r="V47" s="19"/>
+      <c r="W47" s="19"/>
+      <c r="X47" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="29">

</xml_diff>